<commit_message>
TText - added interfacing for (manual!) computations
</commit_message>
<xml_diff>
--- a/TText/TText_Test.xlsx
+++ b/TText/TText_Test.xlsx
@@ -81,9 +81,6 @@
     <t>TText_06</t>
   </si>
   <si>
-    <t>is toegekend</t>
-  </si>
-  <si>
     <t>Piet van der Kluns</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>TText_04</t>
+  </si>
+  <si>
+    <t>ttTopLevel</t>
   </si>
 </sst>
 </file>
@@ -477,21 +477,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.77734375" customWidth="1"/>
-    <col min="2" max="4" width="16.77734375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="52.21875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" customWidth="1"/>
+    <col min="2" max="5" width="16.77734375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="52.21875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -499,140 +499,153 @@
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="2" t="str">
+        <f>$A2</f>
+        <v>TText</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="3" t="str">
+        <f>$A3</f>
+        <v>TText_01</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="F6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="3" t="str">
+        <f>$A7</f>
+        <v>TText_05</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="4"/>
+      <c r="F7" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TText - serious update - includes Scoping, as well as copying/templating. Please read documentation at the beginning of the files.
</commit_message>
<xml_diff>
--- a/TText/TText_Test.xlsx
+++ b/TText/TText_Test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
   <si>
     <t>TText</t>
   </si>
@@ -51,9 +51,6 @@
     <t>[TTexts]</t>
   </si>
   <si>
-    <t>TTScope</t>
-  </si>
-  <si>
     <t>TTValue</t>
   </si>
   <si>
@@ -109,6 +106,57 @@
   </si>
   <si>
     <t>ttTopLevel</t>
+  </si>
+  <si>
+    <t>Scope</t>
+  </si>
+  <si>
+    <t>[Scopes]</t>
+  </si>
+  <si>
+    <t>ScopeID</t>
+  </si>
+  <si>
+    <t>scopeID</t>
+  </si>
+  <si>
+    <t>scopeIsaCasus</t>
+  </si>
+  <si>
+    <t>scopeObject</t>
+  </si>
+  <si>
+    <t>ScopeObject</t>
+  </si>
+  <si>
+    <t>scopeDescription</t>
+  </si>
+  <si>
+    <t>ScopeDescription</t>
+  </si>
+  <si>
+    <t>Zaak_0</t>
+  </si>
+  <si>
+    <t>scopeIncludes</t>
+  </si>
+  <si>
+    <t>ZaakTemplate</t>
+  </si>
+  <si>
+    <t>Schadevergoeding wordt vereist (WA)</t>
+  </si>
+  <si>
+    <t>TText_08</t>
+  </si>
+  <si>
+    <t>TText_09</t>
+  </si>
+  <si>
+    <t>TText_10</t>
+  </si>
+  <si>
+    <t>Klaas Vaak tegen Piet van der Kluns</t>
   </si>
 </sst>
 </file>
@@ -477,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A17" activeCellId="2" sqref="A9 A13 A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,160 +541,293 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="str">
         <f>$A2</f>
-        <v>TText</v>
+        <v>Scope</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="3" t="str">
-        <f>$A3</f>
-        <v>TText_01</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="6" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="C4" s="3" t="str">
+        <f>$A4</f>
+        <v>Zaak_1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>2</v>
+      <c r="C5" s="3" t="str">
+        <f>$A5</f>
+        <v>Zaak_2</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="3" t="str">
-        <f>$A7</f>
-        <v>TText_05</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>4</v>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="2" t="str">
+        <f>$A8</f>
+        <v>TText</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="3" t="str">
+        <f>$A9</f>
+        <v>TText_01</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="F12" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="3" t="str">
+        <f>$A13</f>
+        <v>TText_05</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="E15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="3" t="str">
+        <f>$A17</f>
+        <v>TText_09</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TText - Added SIAM support, and some minor changes.
</commit_message>
<xml_diff>
--- a/TText/TText_Test.xlsx
+++ b/TText/TText_Test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="58">
   <si>
     <t>TText</t>
   </si>
@@ -157,6 +157,39 @@
   </si>
   <si>
     <t>Klaas Vaak tegen Piet van der Kluns</t>
+  </si>
+  <si>
+    <t>[Accounts]</t>
+  </si>
+  <si>
+    <t>accUserid</t>
+  </si>
+  <si>
+    <t>accPassword</t>
+  </si>
+  <si>
+    <t>accPersonRef</t>
+  </si>
+  <si>
+    <t>PersonRef</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Ad Mini Ster</t>
+  </si>
+  <si>
+    <t>autoLoginAccount</t>
   </si>
 </sst>
 </file>
@@ -525,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" activeCellId="2" sqref="A9 A13 A17"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -828,6 +861,61 @@
       </c>
       <c r="F18" s="6" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="2" t="str">
+        <f>$A21</f>
+        <v>Account</v>
+      </c>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="3" t="str">
+        <f>$A22</f>
+        <v>admin</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TText - minor modifications, enhanced interfacing a bit
</commit_message>
<xml_diff>
--- a/TText/TText_Test.xlsx
+++ b/TText/TText_Test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="74">
   <si>
     <t>TText</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Zaak_1</t>
   </si>
   <si>
-    <t>Zaak_2</t>
-  </si>
-  <si>
     <t>TText_04</t>
   </si>
   <si>
@@ -186,10 +183,61 @@
     <t>admin</t>
   </si>
   <si>
-    <t>Ad Mini Ster</t>
-  </si>
-  <si>
     <t>autoLoginAccount</t>
+  </si>
+  <si>
+    <t>toegewezen</t>
+  </si>
+  <si>
+    <t>Ad Minderhout</t>
+  </si>
+  <si>
+    <t>scopeCreateCasusReq</t>
+  </si>
+  <si>
+    <t>Zaak_3</t>
+  </si>
+  <si>
+    <t>Zaak_1A</t>
+  </si>
+  <si>
+    <t>CaseTemplate</t>
+  </si>
+  <si>
+    <t>Case_3</t>
+  </si>
+  <si>
+    <t>Damages ned to be repaired</t>
+  </si>
+  <si>
+    <t>TText_11</t>
+  </si>
+  <si>
+    <t>TText_12</t>
+  </si>
+  <si>
+    <t>Case_0</t>
+  </si>
+  <si>
+    <t>Plaintiff</t>
+  </si>
+  <si>
+    <t>DamageAmount</t>
+  </si>
+  <si>
+    <t>Defendant</t>
+  </si>
+  <si>
+    <t>[Defendant] must pay [DamageAmount] to [Plaintiff]</t>
+  </si>
+  <si>
+    <t>The party that has to defend itself against the claim.</t>
+  </si>
+  <si>
+    <t>The party that has brought the case before the judge.</t>
+  </si>
+  <si>
+    <t>The amount of all damages (in USD)</t>
   </si>
 </sst>
 </file>
@@ -558,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,352 +617,402 @@
     <col min="1" max="1" width="10.77734375" customWidth="1"/>
     <col min="2" max="5" width="16.77734375" style="3" customWidth="1"/>
     <col min="6" max="6" width="52.21875" style="6" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="7" max="7" width="21.21875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="C2" s="2" t="str">
         <f>$A2</f>
         <v>Scope</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="2" t="str">
+        <f>$B2</f>
+        <v>ScopeID</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>39</v>
-      </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" s="3" t="str">
-        <f>$A4</f>
-        <v>Zaak_1</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="C5" s="3" t="str">
         <f>$A5</f>
-        <v>Zaak_2</v>
+        <v>Zaak_1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="2" t="str">
-        <f>$A8</f>
+      <c r="C9" s="2" t="str">
+        <f>$A9</f>
         <v>TText</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="3" t="str">
-        <f>$A9</f>
+      <c r="B10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="3" t="str">
+        <f>$A10</f>
         <v>TText_01</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="6" t="s">
+      <c r="E10" s="4"/>
+      <c r="F10" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="B11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="B12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="3" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>18</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="3" t="str">
-        <f>$A13</f>
-        <v>TText_05</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>19</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="C14" s="3" t="str">
+        <f>$A14</f>
+        <v>TText_05</v>
+      </c>
       <c r="D14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F17" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="3" t="str">
+        <f>$A18</f>
+        <v>TText_09</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="3" t="str">
-        <f>$A17</f>
-        <v>TText_09</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="B19" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E22" s="4"/>
+    </row>
+    <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E26" s="2" t="str">
+        <f>$A26</f>
+        <v>Account</v>
+      </c>
+      <c r="F26" s="5"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="2" t="str">
-        <f>$A21</f>
-        <v>Account</v>
-      </c>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="3" t="str">
-        <f>$A22</f>
+      <c r="E27" s="3" t="str">
+        <f>$A27</f>
         <v>admin</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TText - Major update - renamed several files, relations - introduced ValSuppliers
</commit_message>
<xml_diff>
--- a/TText/TText_Test.xlsx
+++ b/TText/TText_Test.xlsx
@@ -126,12 +126,6 @@
     <t>ScopeObject</t>
   </si>
   <si>
-    <t>scopeDescription</t>
-  </si>
-  <si>
-    <t>ScopeDescription</t>
-  </si>
-  <si>
     <t>Zaak_0</t>
   </si>
   <si>
@@ -238,6 +232,12 @@
   </si>
   <si>
     <t>The amount of all damages (in USD)</t>
+  </si>
+  <si>
+    <t>scopeDescr</t>
+  </si>
+  <si>
+    <t>ScopeDescr</t>
   </si>
 </sst>
 </file>
@@ -608,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -634,13 +634,13 @@
         <v>34</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -661,7 +661,7 @@
         <v>29</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="G2" s="2" t="str">
         <f>$B2</f>
@@ -670,32 +670,32 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -710,13 +710,13 @@
         <v>Zaak_1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -767,7 +767,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" s="3" t="str">
         <f>$A10</f>
@@ -786,7 +786,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>5</v>
@@ -800,7 +800,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>2</v>
@@ -814,7 +814,7 @@
         <v>27</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>23</v>
@@ -838,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>3</v>
@@ -880,7 +880,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>26</v>
@@ -897,10 +897,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C18" s="3" t="str">
         <f>$A18</f>
@@ -911,49 +911,49 @@
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="D20" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="F21" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -961,35 +961,35 @@
     </row>
     <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="E25" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E26" s="2" t="str">
         <f>$A26</f>
@@ -1000,16 +1000,16 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E27" s="3" t="str">
         <f>$A27</f>

</xml_diff>